<commit_message>
Search for subject name is now possible
</commit_message>
<xml_diff>
--- a/interface_shiny/DATA/sub_categories.xlsx
+++ b/interface_shiny/DATA/sub_categories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Activity</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Artwork</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -467,65 +470,94 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ready to be online
</commit_message>
<xml_diff>
--- a/interface_shiny/DATA/sub_categories.xlsx
+++ b/interface_shiny/DATA/sub_categories.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -115,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,37 +442,44 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>